<commit_message>
update report0 & SRS
</commit_message>
<xml_diff>
--- a/Report/Report0_Mapping.xlsx
+++ b/Report/Report0_Mapping.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C010655-817E-4241-B96D-7341D310A57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67809AB6-103A-4BBD-9340-FE3A7D3B517C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>FE-01</t>
   </si>
@@ -91,10 +91,6 @@
     <t>Major Features</t>
   </si>
   <si>
-    <t>Use 
-Cases</t>
-  </si>
-  <si>
     <t>Functional Requirements</t>
   </si>
   <si>
@@ -552,6 +548,21 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>UC-60</t>
+  </si>
+  <si>
+    <t>UC-61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>UC Coverage</t>
   </si>
 </sst>
 </file>
@@ -609,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -632,11 +643,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,11 +675,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -933,24 +975,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DK65"/>
+  <dimension ref="A1:DL65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="16" ySplit="14" topLeftCell="CH51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="16" ySplit="14" topLeftCell="CY15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="CK65" sqref="CK65"/>
+      <selection pane="bottomRight" activeCell="DL22" sqref="DL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="2" max="115" width="6.33203125" customWidth="1"/>
+    <col min="116" max="116" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:116" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>179</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>22</v>
@@ -995,7 +1038,7 @@
       <c r="AN1" s="6"/>
       <c r="AO1" s="6"/>
       <c r="AP1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AQ1" s="6"/>
       <c r="AR1" s="6"/>
@@ -1071,7 +1114,7 @@
       <c r="DJ1" s="6"/>
       <c r="DK1" s="6"/>
     </row>
-    <row r="2" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1101,322 +1144,325 @@
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AP2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BZ2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CF2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="CF2" s="1" t="s">
+      <c r="CG2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="CG2" s="1" t="s">
+      <c r="CH2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="CH2" s="1" t="s">
+      <c r="CI2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="CI2" s="1" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="CJ2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="CK2" s="1" t="s">
+      <c r="CL2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="CL2" s="1" t="s">
+      <c r="CM2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="CM2" s="1" t="s">
+      <c r="CN2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="CN2" s="1" t="s">
+      <c r="CO2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="CO2" s="1" t="s">
+      <c r="CP2" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="CP2" s="1" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="CQ2" s="1" t="s">
+      <c r="CR2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="CR2" s="1" t="s">
+      <c r="CS2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="CS2" s="1" t="s">
+      <c r="CT2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="CT2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="CU2" s="1" t="s">
+      <c r="CV2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="CV2" s="1" t="s">
+      <c r="CW2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="CW2" s="1" t="s">
+      <c r="CX2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="CX2" s="1" t="s">
+      <c r="CY2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="CY2" s="1" t="s">
+      <c r="CZ2" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CZ2" s="1" t="s">
+      <c r="DA2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="DA2" s="1" t="s">
+      <c r="DB2" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="DB2" s="1" t="s">
+      <c r="DC2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="DC2" s="1" t="s">
+      <c r="DD2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="DD2" s="1" t="s">
+      <c r="DE2" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="DE2" s="1" t="s">
+      <c r="DF2" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="DF2" s="1" t="s">
+      <c r="DG2" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="DG2" s="1" t="s">
+      <c r="DH2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="DH2" s="1" t="s">
+      <c r="DI2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="DI2" s="1" t="s">
+      <c r="DJ2" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="DJ2" s="1" t="s">
+      <c r="DK2" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="DK2" s="1" t="s">
-        <v>175</v>
+      <c r="DL2" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1425,7 +1471,9 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1460,7 +1508,9 @@
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
-      <c r="AP3" s="4"/>
+      <c r="AP3" s="4">
+        <v>1</v>
+      </c>
       <c r="AQ3" s="3"/>
       <c r="AR3" s="3"/>
       <c r="AS3" s="3"/>
@@ -1534,12 +1584,18 @@
       <c r="DI3" s="3"/>
       <c r="DJ3" s="3"/>
       <c r="DK3" s="3"/>
+      <c r="DL3">
+        <f>COUNTIF(B3:DK3, 1)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1584,7 +1640,9 @@
       <c r="AR4" s="3"/>
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
-      <c r="AU4" s="4"/>
+      <c r="AU4" s="4">
+        <v>1</v>
+      </c>
       <c r="AV4" s="3"/>
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
@@ -1653,15 +1711,21 @@
       <c r="DI4" s="3"/>
       <c r="DJ4" s="3"/>
       <c r="DK4" s="3"/>
+      <c r="DL4">
+        <f t="shared" ref="DL4:DL63" si="0">COUNTIF(B4:DK4, 1)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1704,7 +1768,9 @@
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="3"/>
-      <c r="AV5" s="4"/>
+      <c r="AV5" s="4">
+        <v>1</v>
+      </c>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
@@ -1772,8 +1838,12 @@
       <c r="DI5" s="3"/>
       <c r="DJ5" s="3"/>
       <c r="DK5" s="3"/>
+      <c r="DL5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1790,7 +1860,9 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -1829,7 +1901,9 @@
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
       <c r="BA6" s="3"/>
-      <c r="BB6" s="4"/>
+      <c r="BB6" s="4">
+        <v>1</v>
+      </c>
       <c r="BC6" s="3"/>
       <c r="BD6" s="3"/>
       <c r="BE6" s="3"/>
@@ -1891,8 +1965,12 @@
       <c r="DI6" s="3"/>
       <c r="DJ6" s="3"/>
       <c r="DK6" s="3"/>
+      <c r="DL6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1900,7 +1978,9 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1943,7 +2023,9 @@
       <c r="AT7" s="3"/>
       <c r="AU7" s="3"/>
       <c r="AV7" s="3"/>
-      <c r="AW7" s="4"/>
+      <c r="AW7" s="4">
+        <v>1</v>
+      </c>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
@@ -2010,8 +2092,12 @@
       <c r="DI7" s="3"/>
       <c r="DJ7" s="3"/>
       <c r="DK7" s="3"/>
+      <c r="DL7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2114,9 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -2067,7 +2155,9 @@
       <c r="AY8" s="3"/>
       <c r="AZ8" s="3"/>
       <c r="BA8" s="3"/>
-      <c r="BB8" s="4"/>
+      <c r="BB8" s="4">
+        <v>1</v>
+      </c>
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
       <c r="BE8" s="3"/>
@@ -2129,14 +2219,20 @@
       <c r="DI8" s="3"/>
       <c r="DJ8" s="3"/>
       <c r="DK8" s="3"/>
+      <c r="DL8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2185,7 +2281,9 @@
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
-      <c r="BA9" s="4"/>
+      <c r="BA9" s="4">
+        <v>1</v>
+      </c>
       <c r="BB9" s="3"/>
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
@@ -2248,8 +2346,12 @@
       <c r="DI9" s="3"/>
       <c r="DJ9" s="3"/>
       <c r="DK9" s="3"/>
+      <c r="DL9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2275,7 +2377,9 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-      <c r="X10" s="4"/>
+      <c r="X10" s="4">
+        <v>1</v>
+      </c>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
@@ -2306,7 +2410,9 @@
       <c r="AZ10" s="3"/>
       <c r="BA10" s="3"/>
       <c r="BB10" s="3"/>
-      <c r="BC10" s="4"/>
+      <c r="BC10" s="4">
+        <v>1</v>
+      </c>
       <c r="BD10" s="3"/>
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
@@ -2367,8 +2473,12 @@
       <c r="DI10" s="3"/>
       <c r="DJ10" s="3"/>
       <c r="DK10" s="3"/>
+      <c r="DL10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2389,7 +2499,9 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="4"/>
+      <c r="S11" s="4">
+        <v>1</v>
+      </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -2421,7 +2533,9 @@
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
-      <c r="AY11" s="4"/>
+      <c r="AY11" s="4">
+        <v>1</v>
+      </c>
       <c r="AZ11" s="3"/>
       <c r="BA11" s="3"/>
       <c r="BB11" s="3"/>
@@ -2486,8 +2600,12 @@
       <c r="DI11" s="3"/>
       <c r="DJ11" s="3"/>
       <c r="DK11" s="3"/>
+      <c r="DL11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2508,7 +2626,9 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="4"/>
+      <c r="S12" s="4">
+        <v>1</v>
+      </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -2546,7 +2666,9 @@
       <c r="BB12" s="3"/>
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
-      <c r="BE12" s="4"/>
+      <c r="BE12" s="4">
+        <v>1</v>
+      </c>
       <c r="BF12" s="3"/>
       <c r="BG12" s="3"/>
       <c r="BH12" s="3"/>
@@ -2605,8 +2727,12 @@
       <c r="DI12" s="3"/>
       <c r="DJ12" s="3"/>
       <c r="DK12" s="3"/>
+      <c r="DL12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2753,9 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="4"/>
+      <c r="S13" s="4">
+        <v>1</v>
+      </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -2659,14 +2787,22 @@
       <c r="AV13" s="3"/>
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
-      <c r="AY13" s="4"/>
+      <c r="AY13" s="4">
+        <v>1</v>
+      </c>
       <c r="AZ13" s="3"/>
       <c r="BA13" s="3"/>
       <c r="BB13" s="3"/>
       <c r="BC13" s="3"/>
-      <c r="BD13" s="4"/>
-      <c r="BE13" s="4"/>
-      <c r="BF13" s="4"/>
+      <c r="BD13" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE13" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF13" s="4">
+        <v>1</v>
+      </c>
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
@@ -2724,8 +2860,12 @@
       <c r="DI13" s="3"/>
       <c r="DJ13" s="3"/>
       <c r="DK13" s="3"/>
+      <c r="DL13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="14" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2746,7 +2886,9 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="4"/>
+      <c r="S14" s="4">
+        <v>1</v>
+      </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -2783,7 +2925,9 @@
       <c r="BA14" s="3"/>
       <c r="BB14" s="3"/>
       <c r="BC14" s="3"/>
-      <c r="BD14" s="4"/>
+      <c r="BD14" s="4">
+        <v>1</v>
+      </c>
       <c r="BE14" s="3"/>
       <c r="BF14" s="3"/>
       <c r="BG14" s="3"/>
@@ -2843,8 +2987,12 @@
       <c r="DI14" s="3"/>
       <c r="DJ14" s="3"/>
       <c r="DK14" s="3"/>
+      <c r="DL14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2865,7 +3013,9 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="4">
+        <v>1</v>
+      </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -2904,7 +3054,9 @@
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
       <c r="BE15" s="3"/>
-      <c r="BF15" s="4"/>
+      <c r="BF15" s="4">
+        <v>1</v>
+      </c>
       <c r="BG15" s="3"/>
       <c r="BH15" s="3"/>
       <c r="BI15" s="3"/>
@@ -2962,10 +3114,14 @@
       <c r="DI15" s="3"/>
       <c r="DJ15" s="3"/>
       <c r="DK15" s="3"/>
+      <c r="DL15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2988,7 +3144,9 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="4"/>
+      <c r="W16" s="4">
+        <v>1</v>
+      </c>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -3034,7 +3192,9 @@
       <c r="BN16" s="3"/>
       <c r="BO16" s="3"/>
       <c r="BP16" s="3"/>
-      <c r="BQ16" s="4"/>
+      <c r="BQ16" s="4">
+        <v>1</v>
+      </c>
       <c r="BR16" s="3"/>
       <c r="BS16" s="3"/>
       <c r="BT16" s="3"/>
@@ -3081,10 +3241,14 @@
       <c r="DI16" s="3"/>
       <c r="DJ16" s="3"/>
       <c r="DK16" s="3"/>
+      <c r="DL16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3101,7 +3265,9 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="4"/>
+      <c r="Q17" s="4">
+        <v>1</v>
+      </c>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -3143,7 +3309,9 @@
       <c r="BD17" s="3"/>
       <c r="BE17" s="3"/>
       <c r="BF17" s="3"/>
-      <c r="BG17" s="4"/>
+      <c r="BG17" s="4">
+        <v>1</v>
+      </c>
       <c r="BH17" s="3"/>
       <c r="BI17" s="3"/>
       <c r="BJ17" s="3"/>
@@ -3200,10 +3368,14 @@
       <c r="DI17" s="3"/>
       <c r="DJ17" s="3"/>
       <c r="DK17" s="3"/>
+      <c r="DL17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3225,7 +3397,9 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="4"/>
+      <c r="V18" s="4">
+        <v>1</v>
+      </c>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
@@ -3264,7 +3438,9 @@
       <c r="BF18" s="3"/>
       <c r="BG18" s="3"/>
       <c r="BH18" s="3"/>
-      <c r="BI18" s="4"/>
+      <c r="BI18" s="4">
+        <v>1</v>
+      </c>
       <c r="BJ18" s="3"/>
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
@@ -3319,10 +3495,14 @@
       <c r="DI18" s="3"/>
       <c r="DJ18" s="3"/>
       <c r="DK18" s="3"/>
+      <c r="DL18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3334,7 +3514,9 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -3384,7 +3566,9 @@
       <c r="BG19" s="3"/>
       <c r="BH19" s="3"/>
       <c r="BI19" s="3"/>
-      <c r="BJ19" s="4"/>
+      <c r="BJ19" s="4">
+        <v>1</v>
+      </c>
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
@@ -3438,10 +3622,14 @@
       <c r="DI19" s="3"/>
       <c r="DJ19" s="3"/>
       <c r="DK19" s="3"/>
+      <c r="DL19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3452,7 +3640,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -3506,8 +3696,12 @@
       <c r="BJ20" s="3"/>
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
-      <c r="BM20" s="4"/>
-      <c r="BN20" s="4"/>
+      <c r="BM20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN20" s="4">
+        <v>1</v>
+      </c>
       <c r="BO20" s="3"/>
       <c r="BP20" s="3"/>
       <c r="BQ20" s="3"/>
@@ -3557,10 +3751,14 @@
       <c r="DI20" s="3"/>
       <c r="DJ20" s="3"/>
       <c r="DK20" s="3"/>
+      <c r="DL20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3581,7 +3779,9 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="4"/>
+      <c r="U21" s="4">
+        <v>1</v>
+      </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -3676,10 +3876,14 @@
       <c r="DI21" s="3"/>
       <c r="DJ21" s="3"/>
       <c r="DK21" s="3"/>
+      <c r="DL21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3795,10 +3999,14 @@
       <c r="DI22" s="3"/>
       <c r="DJ22" s="3"/>
       <c r="DK22" s="3"/>
+      <c r="DL22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3808,7 +4016,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -3864,7 +4074,9 @@
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
       <c r="BM23" s="3"/>
-      <c r="BN23" s="4"/>
+      <c r="BN23" s="4">
+        <v>1</v>
+      </c>
       <c r="BO23" s="3"/>
       <c r="BP23" s="3"/>
       <c r="BQ23" s="3"/>
@@ -3914,10 +4126,14 @@
       <c r="DI23" s="3"/>
       <c r="DJ23" s="3"/>
       <c r="DK23" s="3"/>
+      <c r="DL23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3930,7 +4146,9 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -4033,10 +4251,14 @@
       <c r="DI24" s="3"/>
       <c r="DJ24" s="3"/>
       <c r="DK24" s="3"/>
+      <c r="DL24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4062,7 +4284,9 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="4"/>
+      <c r="Z25" s="4">
+        <v>1</v>
+      </c>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
@@ -4090,7 +4314,9 @@
       <c r="AY25" s="3"/>
       <c r="AZ25" s="3"/>
       <c r="BA25" s="3"/>
-      <c r="BB25" s="4"/>
+      <c r="BB25" s="4">
+        <v>1</v>
+      </c>
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
       <c r="BE25" s="3"/>
@@ -4152,10 +4378,14 @@
       <c r="DI25" s="3"/>
       <c r="DJ25" s="3"/>
       <c r="DK25" s="3"/>
+      <c r="DL25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4181,7 +4411,9 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="4"/>
+      <c r="Z26" s="4">
+        <v>1</v>
+      </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
@@ -4209,7 +4441,9 @@
       <c r="AY26" s="3"/>
       <c r="AZ26" s="3"/>
       <c r="BA26" s="3"/>
-      <c r="BB26" s="4"/>
+      <c r="BB26" s="4">
+        <v>1</v>
+      </c>
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
       <c r="BE26" s="3"/>
@@ -4271,10 +4505,14 @@
       <c r="DI26" s="3"/>
       <c r="DJ26" s="3"/>
       <c r="DK26" s="3"/>
+      <c r="DL26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="27" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4309,7 +4547,9 @@
       <c r="AF27" s="3"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
-      <c r="AI27" s="4"/>
+      <c r="AI27" s="4">
+        <v>1</v>
+      </c>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
       <c r="AL27" s="3"/>
@@ -4362,11 +4602,21 @@
       <c r="CG27" s="3"/>
       <c r="CH27" s="3"/>
       <c r="CI27" s="3"/>
-      <c r="CJ27" s="5"/>
-      <c r="CK27" s="4"/>
-      <c r="CL27" s="4"/>
-      <c r="CM27" s="4"/>
-      <c r="CN27" s="5"/>
+      <c r="CJ27" s="5">
+        <v>1</v>
+      </c>
+      <c r="CK27" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL27" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM27" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN27" s="5">
+        <v>1</v>
+      </c>
       <c r="CO27" s="3"/>
       <c r="CP27" s="3"/>
       <c r="CQ27" s="3"/>
@@ -4390,13 +4640,19 @@
       <c r="DI27" s="3"/>
       <c r="DJ27" s="3"/>
       <c r="DK27" s="3"/>
+      <c r="DL27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -4466,8 +4722,12 @@
       <c r="BR28" s="3"/>
       <c r="BS28" s="3"/>
       <c r="BT28" s="3"/>
-      <c r="BU28" s="4"/>
-      <c r="BV28" s="4"/>
+      <c r="BU28" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV28" s="4">
+        <v>1</v>
+      </c>
       <c r="BW28" s="3"/>
       <c r="BX28" s="3"/>
       <c r="BY28" s="3"/>
@@ -4509,10 +4769,14 @@
       <c r="DI28" s="3"/>
       <c r="DJ28" s="3"/>
       <c r="DK28" s="3"/>
+      <c r="DL28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="29" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4547,7 +4811,9 @@
       <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
-      <c r="AI29" s="4"/>
+      <c r="AI29" s="4">
+        <v>1</v>
+      </c>
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
       <c r="AL29" s="3"/>
@@ -4601,7 +4867,9 @@
       <c r="CH29" s="3"/>
       <c r="CI29" s="3"/>
       <c r="CJ29" s="3"/>
-      <c r="CK29" s="4"/>
+      <c r="CK29" s="4">
+        <v>1</v>
+      </c>
       <c r="CL29" s="3"/>
       <c r="CM29" s="3"/>
       <c r="CN29" s="3"/>
@@ -4628,10 +4896,14 @@
       <c r="DI29" s="3"/>
       <c r="DJ29" s="3"/>
       <c r="DK29" s="3"/>
+      <c r="DL29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="30" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4666,7 +4938,9 @@
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
-      <c r="AI30" s="4"/>
+      <c r="AI30" s="4">
+        <v>1</v>
+      </c>
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
@@ -4722,7 +4996,9 @@
       <c r="CJ30" s="3"/>
       <c r="CK30" s="3"/>
       <c r="CL30" s="3"/>
-      <c r="CM30" s="4"/>
+      <c r="CM30" s="4">
+        <v>1</v>
+      </c>
       <c r="CN30" s="3"/>
       <c r="CO30" s="3"/>
       <c r="CP30" s="3"/>
@@ -4747,10 +5023,14 @@
       <c r="DI30" s="3"/>
       <c r="DJ30" s="3"/>
       <c r="DK30" s="3"/>
+      <c r="DL30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="31" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4786,7 +5066,9 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
-      <c r="AJ31" s="4"/>
+      <c r="AJ31" s="4">
+        <v>1</v>
+      </c>
       <c r="AK31" s="3"/>
       <c r="AL31" s="3"/>
       <c r="AM31" s="3"/>
@@ -4866,10 +5148,14 @@
       <c r="DI31" s="3"/>
       <c r="DJ31" s="3"/>
       <c r="DK31" s="3"/>
+      <c r="DL31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4892,7 +5178,9 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
-      <c r="W32" s="4"/>
+      <c r="W32" s="4">
+        <v>1</v>
+      </c>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
@@ -4938,7 +5226,9 @@
       <c r="BN32" s="3"/>
       <c r="BO32" s="3"/>
       <c r="BP32" s="3"/>
-      <c r="BQ32" s="4"/>
+      <c r="BQ32" s="4">
+        <v>1</v>
+      </c>
       <c r="BR32" s="3"/>
       <c r="BS32" s="3"/>
       <c r="BT32" s="3"/>
@@ -4985,10 +5275,14 @@
       <c r="DI32" s="3"/>
       <c r="DJ32" s="3"/>
       <c r="DK32" s="3"/>
+      <c r="DL32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="33" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5024,7 +5318,9 @@
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
-      <c r="AJ33" s="4"/>
+      <c r="AJ33" s="4">
+        <v>1</v>
+      </c>
       <c r="AK33" s="3"/>
       <c r="AL33" s="3"/>
       <c r="AM33" s="3"/>
@@ -5104,10 +5400,14 @@
       <c r="DI33" s="3"/>
       <c r="DJ33" s="3"/>
       <c r="DK33" s="3"/>
+      <c r="DL33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5145,7 +5445,9 @@
       <c r="AI34" s="3"/>
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
-      <c r="AL34" s="4"/>
+      <c r="AL34" s="4">
+        <v>1</v>
+      </c>
       <c r="AM34" s="3"/>
       <c r="AN34" s="3"/>
       <c r="AO34" s="3"/>
@@ -5168,7 +5470,9 @@
       <c r="BF34" s="3"/>
       <c r="BG34" s="3"/>
       <c r="BH34" s="3"/>
-      <c r="BI34" s="4"/>
+      <c r="BI34" s="4">
+        <v>1</v>
+      </c>
       <c r="BJ34" s="3"/>
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
@@ -5182,7 +5486,9 @@
       <c r="BT34" s="3"/>
       <c r="BU34" s="3"/>
       <c r="BV34" s="3"/>
-      <c r="BW34" s="4"/>
+      <c r="BW34" s="4">
+        <v>1</v>
+      </c>
       <c r="BX34" s="3"/>
       <c r="BY34" s="3"/>
       <c r="BZ34" s="3"/>
@@ -5223,10 +5529,14 @@
       <c r="DI34" s="3"/>
       <c r="DJ34" s="3"/>
       <c r="DK34" s="3"/>
+      <c r="DL34">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="35" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5265,7 +5575,9 @@
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
-      <c r="AM35" s="4"/>
+      <c r="AM35" s="4">
+        <v>1</v>
+      </c>
       <c r="AN35" s="3"/>
       <c r="AO35" s="3"/>
       <c r="AP35" s="3"/>
@@ -5310,7 +5622,9 @@
       <c r="CC35" s="3"/>
       <c r="CD35" s="3"/>
       <c r="CE35" s="3"/>
-      <c r="CF35" s="4"/>
+      <c r="CF35" s="4">
+        <v>1</v>
+      </c>
       <c r="CG35" s="3"/>
       <c r="CH35" s="3"/>
       <c r="CI35" s="3"/>
@@ -5342,10 +5656,14 @@
       <c r="DI35" s="3"/>
       <c r="DJ35" s="3"/>
       <c r="DK35" s="3"/>
+      <c r="DL35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="36" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5374,7 +5692,9 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
-      <c r="AC36" s="4"/>
+      <c r="AC36" s="4">
+        <v>1</v>
+      </c>
       <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
@@ -5420,7 +5740,9 @@
       <c r="BT36" s="3"/>
       <c r="BU36" s="3"/>
       <c r="BV36" s="3"/>
-      <c r="BW36" s="4"/>
+      <c r="BW36" s="4">
+        <v>1</v>
+      </c>
       <c r="BX36" s="3"/>
       <c r="BY36" s="3"/>
       <c r="BZ36" s="3"/>
@@ -5451,7 +5773,9 @@
       <c r="CY36" s="3"/>
       <c r="CZ36" s="3"/>
       <c r="DA36" s="3"/>
-      <c r="DB36" s="3"/>
+      <c r="DB36" s="4">
+        <v>1</v>
+      </c>
       <c r="DC36" s="3"/>
       <c r="DD36" s="3"/>
       <c r="DE36" s="3"/>
@@ -5461,10 +5785,14 @@
       <c r="DI36" s="3"/>
       <c r="DJ36" s="3"/>
       <c r="DK36" s="3"/>
+      <c r="DL36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="37" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5497,7 +5825,9 @@
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
-      <c r="AG37" s="4"/>
+      <c r="AG37" s="4">
+        <v>1</v>
+      </c>
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
@@ -5580,10 +5910,14 @@
       <c r="DI37" s="3"/>
       <c r="DJ37" s="3"/>
       <c r="DK37" s="3"/>
+      <c r="DL37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5611,7 +5945,9 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
-      <c r="AB38" s="4"/>
+      <c r="AB38" s="4">
+        <v>1</v>
+      </c>
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
@@ -5683,7 +6019,9 @@
       <c r="CS38" s="3"/>
       <c r="CT38" s="3"/>
       <c r="CU38" s="3"/>
-      <c r="CV38" s="4"/>
+      <c r="CV38" s="4">
+        <v>1</v>
+      </c>
       <c r="CW38" s="3"/>
       <c r="CX38" s="3"/>
       <c r="CY38" s="3"/>
@@ -5699,10 +6037,14 @@
       <c r="DI38" s="3"/>
       <c r="DJ38" s="3"/>
       <c r="DK38" s="3"/>
+      <c r="DL38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5730,7 +6072,9 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
-      <c r="AB39" s="4"/>
+      <c r="AB39" s="4">
+        <v>1</v>
+      </c>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
       <c r="AE39" s="3"/>
@@ -5806,7 +6150,9 @@
       <c r="CW39" s="3"/>
       <c r="CX39" s="3"/>
       <c r="CY39" s="3"/>
-      <c r="CZ39" s="4"/>
+      <c r="CZ39" s="4">
+        <v>1</v>
+      </c>
       <c r="DA39" s="3"/>
       <c r="DB39" s="3"/>
       <c r="DC39" s="3"/>
@@ -5818,10 +6164,14 @@
       <c r="DI39" s="3"/>
       <c r="DJ39" s="3"/>
       <c r="DK39" s="3"/>
+      <c r="DL39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5849,7 +6199,9 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
-      <c r="AB40" s="4"/>
+      <c r="AB40" s="4">
+        <v>1</v>
+      </c>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
       <c r="AE40" s="3"/>
@@ -5924,7 +6276,9 @@
       <c r="CV40" s="3"/>
       <c r="CW40" s="3"/>
       <c r="CX40" s="3"/>
-      <c r="CY40" s="4"/>
+      <c r="CY40" s="4">
+        <v>1</v>
+      </c>
       <c r="CZ40" s="3"/>
       <c r="DA40" s="3"/>
       <c r="DB40" s="3"/>
@@ -5937,10 +6291,14 @@
       <c r="DI40" s="3"/>
       <c r="DJ40" s="3"/>
       <c r="DK40" s="3"/>
+      <c r="DL40">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="41" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5968,7 +6326,9 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
-      <c r="AB41" s="4"/>
+      <c r="AB41" s="4">
+        <v>1</v>
+      </c>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
@@ -6039,12 +6399,20 @@
       <c r="CR41" s="3"/>
       <c r="CS41" s="3"/>
       <c r="CT41" s="3"/>
-      <c r="CU41" s="4"/>
-      <c r="CV41" s="4"/>
-      <c r="CW41" s="4"/>
+      <c r="CU41" s="4">
+        <v>1</v>
+      </c>
+      <c r="CV41" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW41" s="4">
+        <v>1</v>
+      </c>
       <c r="CX41" s="3"/>
       <c r="CY41" s="3"/>
-      <c r="CZ41" s="4"/>
+      <c r="CZ41" s="4">
+        <v>1</v>
+      </c>
       <c r="DA41" s="3"/>
       <c r="DB41" s="3"/>
       <c r="DC41" s="3"/>
@@ -6056,10 +6424,14 @@
       <c r="DI41" s="3"/>
       <c r="DJ41" s="3"/>
       <c r="DK41" s="3"/>
+      <c r="DL41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6093,7 +6465,9 @@
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
       <c r="AG42" s="3"/>
-      <c r="AH42" s="4"/>
+      <c r="AH42" s="4">
+        <v>1</v>
+      </c>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -6161,7 +6535,9 @@
       <c r="CU42" s="3"/>
       <c r="CV42" s="3"/>
       <c r="CW42" s="3"/>
-      <c r="CX42" s="4"/>
+      <c r="CX42" s="4">
+        <v>1</v>
+      </c>
       <c r="CY42" s="3"/>
       <c r="CZ42" s="3"/>
       <c r="DA42" s="3"/>
@@ -6175,10 +6551,14 @@
       <c r="DI42" s="3"/>
       <c r="DJ42" s="3"/>
       <c r="DK42" s="3"/>
+      <c r="DL42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6210,7 +6590,9 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
       <c r="AE43" s="3"/>
-      <c r="AF43" s="4"/>
+      <c r="AF43" s="4">
+        <v>1</v>
+      </c>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
@@ -6294,10 +6676,14 @@
       <c r="DI43" s="3"/>
       <c r="DJ43" s="3"/>
       <c r="DK43" s="3"/>
+      <c r="DL43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -6336,7 +6722,9 @@
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
-      <c r="AM44" s="4"/>
+      <c r="AM44" s="4">
+        <v>1</v>
+      </c>
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
@@ -6381,7 +6769,9 @@
       <c r="CC44" s="3"/>
       <c r="CD44" s="3"/>
       <c r="CE44" s="3"/>
-      <c r="CF44" s="4"/>
+      <c r="CF44" s="4">
+        <v>1</v>
+      </c>
       <c r="CG44" s="3"/>
       <c r="CH44" s="3"/>
       <c r="CI44" s="3"/>
@@ -6413,10 +6803,14 @@
       <c r="DI44" s="3"/>
       <c r="DJ44" s="3"/>
       <c r="DK44" s="3"/>
+      <c r="DL44">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="45" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -6453,7 +6847,9 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
-      <c r="AK45" s="4"/>
+      <c r="AK45" s="4">
+        <v>1</v>
+      </c>
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
       <c r="AN45" s="3"/>
@@ -6481,8 +6877,12 @@
       <c r="BJ45" s="3"/>
       <c r="BK45" s="3"/>
       <c r="BL45" s="3"/>
-      <c r="BM45" s="4"/>
-      <c r="BN45" s="4"/>
+      <c r="BM45" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN45" s="4">
+        <v>1</v>
+      </c>
       <c r="BO45" s="3"/>
       <c r="BP45" s="3"/>
       <c r="BQ45" s="3"/>
@@ -6532,10 +6932,14 @@
       <c r="DI45" s="3"/>
       <c r="DJ45" s="3"/>
       <c r="DK45" s="3"/>
+      <c r="DL45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="46" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -6567,7 +6971,9 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
       <c r="AE46" s="3"/>
-      <c r="AF46" s="4"/>
+      <c r="AF46" s="4">
+        <v>1</v>
+      </c>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
@@ -6643,18 +7049,32 @@
       <c r="DA46" s="3"/>
       <c r="DB46" s="3"/>
       <c r="DC46" s="3"/>
-      <c r="DD46" s="3"/>
-      <c r="DE46" s="3"/>
-      <c r="DF46" s="3"/>
-      <c r="DG46" s="3"/>
+      <c r="DD46" s="4">
+        <v>1</v>
+      </c>
+      <c r="DE46" s="4">
+        <v>1</v>
+      </c>
+      <c r="DF46" s="4">
+        <v>1</v>
+      </c>
+      <c r="DG46" s="4">
+        <v>1</v>
+      </c>
       <c r="DH46" s="3"/>
-      <c r="DI46" s="3"/>
+      <c r="DI46" s="4">
+        <v>1</v>
+      </c>
       <c r="DJ46" s="3"/>
       <c r="DK46" s="3"/>
+      <c r="DL46">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="47" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -6664,7 +7084,9 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="4"/>
+      <c r="J47" s="4">
+        <v>1</v>
+      </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -6720,7 +7142,9 @@
       <c r="BK47" s="3"/>
       <c r="BL47" s="3"/>
       <c r="BM47" s="3"/>
-      <c r="BN47" s="4"/>
+      <c r="BN47" s="4">
+        <v>1</v>
+      </c>
       <c r="BO47" s="3"/>
       <c r="BP47" s="3"/>
       <c r="BQ47" s="3"/>
@@ -6770,10 +7194,14 @@
       <c r="DI47" s="3"/>
       <c r="DJ47" s="3"/>
       <c r="DK47" s="3"/>
+      <c r="DL47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="48" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -6805,7 +7233,9 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
-      <c r="AF48" s="4"/>
+      <c r="AF48" s="4">
+        <v>1</v>
+      </c>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
@@ -6889,10 +7319,14 @@
       <c r="DI48" s="3"/>
       <c r="DJ48" s="3"/>
       <c r="DK48" s="3"/>
+      <c r="DL48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -6919,7 +7353,9 @@
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
-      <c r="AA49" s="4"/>
+      <c r="AA49" s="4">
+        <v>1</v>
+      </c>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
@@ -6960,7 +7396,9 @@
       <c r="BM49" s="3"/>
       <c r="BN49" s="3"/>
       <c r="BO49" s="3"/>
-      <c r="BP49" s="4"/>
+      <c r="BP49" s="4">
+        <v>1</v>
+      </c>
       <c r="BQ49" s="3"/>
       <c r="BR49" s="3"/>
       <c r="BS49" s="3"/>
@@ -7004,14 +7442,20 @@
       <c r="DE49" s="3"/>
       <c r="DF49" s="3"/>
       <c r="DG49" s="3"/>
-      <c r="DH49" s="3"/>
+      <c r="DH49" s="4">
+        <v>1</v>
+      </c>
       <c r="DI49" s="3"/>
       <c r="DJ49" s="3"/>
       <c r="DK49" s="3"/>
+      <c r="DL49">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="50" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -7038,7 +7482,9 @@
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
-      <c r="AA50" s="4"/>
+      <c r="AA50" s="4">
+        <v>1</v>
+      </c>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
@@ -7123,14 +7569,20 @@
       <c r="DE50" s="3"/>
       <c r="DF50" s="3"/>
       <c r="DG50" s="3"/>
-      <c r="DH50" s="3"/>
+      <c r="DH50" s="4">
+        <v>1</v>
+      </c>
       <c r="DI50" s="3"/>
       <c r="DJ50" s="3"/>
       <c r="DK50" s="3"/>
+      <c r="DL50">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="51" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -7170,7 +7622,9 @@
       <c r="AK51" s="3"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="3"/>
-      <c r="AN51" s="4"/>
+      <c r="AN51" s="4">
+        <v>1</v>
+      </c>
       <c r="AO51" s="3"/>
       <c r="AP51" s="3"/>
       <c r="AQ51" s="3"/>
@@ -7206,10 +7660,16 @@
       <c r="BU51" s="3"/>
       <c r="BV51" s="3"/>
       <c r="BW51" s="3"/>
-      <c r="BX51" s="4"/>
-      <c r="BY51" s="3"/>
+      <c r="BX51" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY51" s="4">
+        <v>1</v>
+      </c>
       <c r="BZ51" s="3"/>
-      <c r="CA51" s="4"/>
+      <c r="CA51" s="4">
+        <v>1</v>
+      </c>
       <c r="CB51" s="3"/>
       <c r="CC51" s="3"/>
       <c r="CD51" s="3"/>
@@ -7246,10 +7706,14 @@
       <c r="DI51" s="3"/>
       <c r="DJ51" s="3"/>
       <c r="DK51" s="3"/>
+      <c r="DL51">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -7289,7 +7753,9 @@
       <c r="AK52" s="3"/>
       <c r="AL52" s="3"/>
       <c r="AM52" s="3"/>
-      <c r="AN52" s="4"/>
+      <c r="AN52" s="4">
+        <v>1</v>
+      </c>
       <c r="AO52" s="3"/>
       <c r="AP52" s="3"/>
       <c r="AQ52" s="3"/>
@@ -7331,7 +7797,9 @@
       <c r="CA52" s="3"/>
       <c r="CB52" s="3"/>
       <c r="CC52" s="3"/>
-      <c r="CD52" s="4"/>
+      <c r="CD52" s="4">
+        <v>1</v>
+      </c>
       <c r="CE52" s="3"/>
       <c r="CF52" s="3"/>
       <c r="CG52" s="3"/>
@@ -7365,10 +7833,14 @@
       <c r="DI52" s="3"/>
       <c r="DJ52" s="3"/>
       <c r="DK52" s="3"/>
+      <c r="DL52">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="53" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -7387,7 +7859,9 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
-      <c r="S53" s="4"/>
+      <c r="S53" s="4">
+        <v>1</v>
+      </c>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
@@ -7424,9 +7898,13 @@
       <c r="BA53" s="3"/>
       <c r="BB53" s="3"/>
       <c r="BC53" s="3"/>
-      <c r="BD53" s="4"/>
+      <c r="BD53" s="4">
+        <v>1</v>
+      </c>
       <c r="BE53" s="3"/>
-      <c r="BF53" s="4"/>
+      <c r="BF53" s="4">
+        <v>1</v>
+      </c>
       <c r="BG53" s="3"/>
       <c r="BH53" s="3"/>
       <c r="BI53" s="3"/>
@@ -7484,10 +7962,14 @@
       <c r="DI53" s="3"/>
       <c r="DJ53" s="3"/>
       <c r="DK53" s="3"/>
+      <c r="DL53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="54" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -7527,7 +8009,9 @@
       <c r="AK54" s="3"/>
       <c r="AL54" s="3"/>
       <c r="AM54" s="3"/>
-      <c r="AN54" s="4"/>
+      <c r="AN54" s="4">
+        <v>1</v>
+      </c>
       <c r="AO54" s="3"/>
       <c r="AP54" s="3"/>
       <c r="AQ54" s="3"/>
@@ -7568,9 +8052,13 @@
       <c r="BZ54" s="3"/>
       <c r="CA54" s="3"/>
       <c r="CB54" s="3"/>
-      <c r="CC54" s="4"/>
+      <c r="CC54" s="4">
+        <v>1</v>
+      </c>
       <c r="CD54" s="3"/>
-      <c r="CE54" s="4"/>
+      <c r="CE54" s="4">
+        <v>1</v>
+      </c>
       <c r="CF54" s="3"/>
       <c r="CG54" s="3"/>
       <c r="CH54" s="3"/>
@@ -7603,10 +8091,14 @@
       <c r="DI54" s="3"/>
       <c r="DJ54" s="3"/>
       <c r="DK54" s="3"/>
+      <c r="DL54">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="55" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -7647,7 +8139,9 @@
       <c r="AL55" s="3"/>
       <c r="AM55" s="3"/>
       <c r="AN55" s="3"/>
-      <c r="AO55" s="4"/>
+      <c r="AO55" s="4">
+        <v>1</v>
+      </c>
       <c r="AP55" s="3"/>
       <c r="AQ55" s="3"/>
       <c r="AR55" s="3"/>
@@ -7691,7 +8185,9 @@
       <c r="CD55" s="3"/>
       <c r="CE55" s="3"/>
       <c r="CF55" s="3"/>
-      <c r="CG55" s="4"/>
+      <c r="CG55" s="4">
+        <v>1</v>
+      </c>
       <c r="CH55" s="3"/>
       <c r="CI55" s="3"/>
       <c r="CJ55" s="3"/>
@@ -7722,10 +8218,14 @@
       <c r="DI55" s="3"/>
       <c r="DJ55" s="3"/>
       <c r="DK55" s="3"/>
+      <c r="DL55">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="56" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -7766,7 +8266,9 @@
       <c r="AL56" s="3"/>
       <c r="AM56" s="3"/>
       <c r="AN56" s="3"/>
-      <c r="AO56" s="4"/>
+      <c r="AO56" s="4">
+        <v>1</v>
+      </c>
       <c r="AP56" s="3"/>
       <c r="AQ56" s="3"/>
       <c r="AR56" s="3"/>
@@ -7810,7 +8312,9 @@
       <c r="CD56" s="3"/>
       <c r="CE56" s="3"/>
       <c r="CF56" s="3"/>
-      <c r="CG56" s="4"/>
+      <c r="CG56" s="4">
+        <v>1</v>
+      </c>
       <c r="CH56" s="3"/>
       <c r="CI56" s="3"/>
       <c r="CJ56" s="3"/>
@@ -7841,10 +8345,14 @@
       <c r="DI56" s="3"/>
       <c r="DJ56" s="3"/>
       <c r="DK56" s="3"/>
+      <c r="DL56">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="57" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -7885,7 +8393,9 @@
       <c r="AL57" s="3"/>
       <c r="AM57" s="3"/>
       <c r="AN57" s="3"/>
-      <c r="AO57" s="4"/>
+      <c r="AO57" s="4">
+        <v>1</v>
+      </c>
       <c r="AP57" s="3"/>
       <c r="AQ57" s="3"/>
       <c r="AR57" s="3"/>
@@ -7929,7 +8439,9 @@
       <c r="CD57" s="3"/>
       <c r="CE57" s="3"/>
       <c r="CF57" s="3"/>
-      <c r="CG57" s="4"/>
+      <c r="CG57" s="4">
+        <v>1</v>
+      </c>
       <c r="CH57" s="3"/>
       <c r="CI57" s="3"/>
       <c r="CJ57" s="3"/>
@@ -7960,10 +8472,14 @@
       <c r="DI57" s="3"/>
       <c r="DJ57" s="3"/>
       <c r="DK57" s="3"/>
+      <c r="DL57">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -8004,7 +8520,9 @@
       <c r="AL58" s="3"/>
       <c r="AM58" s="3"/>
       <c r="AN58" s="3"/>
-      <c r="AO58" s="4"/>
+      <c r="AO58" s="4">
+        <v>1</v>
+      </c>
       <c r="AP58" s="3"/>
       <c r="AQ58" s="3"/>
       <c r="AR58" s="3"/>
@@ -8048,7 +8566,9 @@
       <c r="CD58" s="3"/>
       <c r="CE58" s="3"/>
       <c r="CF58" s="3"/>
-      <c r="CG58" s="4"/>
+      <c r="CG58" s="4">
+        <v>1</v>
+      </c>
       <c r="CH58" s="3"/>
       <c r="CI58" s="3"/>
       <c r="CJ58" s="3"/>
@@ -8079,10 +8599,14 @@
       <c r="DI58" s="3"/>
       <c r="DJ58" s="3"/>
       <c r="DK58" s="3"/>
+      <c r="DL58">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="59" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -8123,7 +8647,9 @@
       <c r="AL59" s="3"/>
       <c r="AM59" s="3"/>
       <c r="AN59" s="3"/>
-      <c r="AO59" s="4"/>
+      <c r="AO59" s="4">
+        <v>1</v>
+      </c>
       <c r="AP59" s="3"/>
       <c r="AQ59" s="3"/>
       <c r="AR59" s="3"/>
@@ -8167,7 +8693,9 @@
       <c r="CD59" s="3"/>
       <c r="CE59" s="3"/>
       <c r="CF59" s="3"/>
-      <c r="CG59" s="4"/>
+      <c r="CG59" s="4">
+        <v>1</v>
+      </c>
       <c r="CH59" s="3"/>
       <c r="CI59" s="3"/>
       <c r="CJ59" s="3"/>
@@ -8198,17 +8726,23 @@
       <c r="DI59" s="3"/>
       <c r="DJ59" s="3"/>
       <c r="DK59" s="3"/>
+      <c r="DL59">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="4"/>
+      <c r="G60" s="4">
+        <v>1</v>
+      </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
@@ -8244,7 +8778,9 @@
       <c r="AN60" s="3"/>
       <c r="AO60" s="3"/>
       <c r="AP60" s="3"/>
-      <c r="AQ60" s="4"/>
+      <c r="AQ60" s="4">
+        <v>1</v>
+      </c>
       <c r="AR60" s="3"/>
       <c r="AS60" s="3"/>
       <c r="AT60" s="3"/>
@@ -8276,7 +8812,9 @@
       <c r="BT60" s="3"/>
       <c r="BU60" s="3"/>
       <c r="BV60" s="3"/>
-      <c r="BW60" s="4"/>
+      <c r="BW60" s="4">
+        <v>1</v>
+      </c>
       <c r="BX60" s="3"/>
       <c r="BY60" s="3"/>
       <c r="BZ60" s="3"/>
@@ -8287,7 +8825,9 @@
       <c r="CE60" s="3"/>
       <c r="CF60" s="3"/>
       <c r="CG60" s="3"/>
-      <c r="CH60" s="4"/>
+      <c r="CH60" s="4">
+        <v>1</v>
+      </c>
       <c r="CI60" s="3"/>
       <c r="CJ60" s="3"/>
       <c r="CK60" s="3"/>
@@ -8317,17 +8857,23 @@
       <c r="DI60" s="3"/>
       <c r="DJ60" s="3"/>
       <c r="DK60" s="3"/>
+      <c r="DL60">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="4"/>
+      <c r="G61" s="4">
+        <v>1</v>
+      </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
@@ -8436,10 +8982,274 @@
       <c r="DI61" s="3"/>
       <c r="DJ61" s="3"/>
       <c r="DK61" s="3"/>
+      <c r="DL61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:116" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3"/>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3"/>
+      <c r="AC62" s="3"/>
+      <c r="AD62" s="3"/>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3"/>
+      <c r="AK62" s="3"/>
+      <c r="AL62" s="3"/>
+      <c r="AM62" s="3"/>
+      <c r="AN62" s="3"/>
+      <c r="AO62" s="3"/>
+      <c r="AP62" s="3"/>
+      <c r="AQ62" s="3"/>
+      <c r="AR62" s="3"/>
+      <c r="AS62" s="3"/>
+      <c r="AT62" s="3"/>
+      <c r="AU62" s="3"/>
+      <c r="AV62" s="3"/>
+      <c r="AW62" s="3"/>
+      <c r="AX62" s="3"/>
+      <c r="AY62" s="3"/>
+      <c r="AZ62" s="3"/>
+      <c r="BA62" s="3"/>
+      <c r="BB62" s="3"/>
+      <c r="BC62" s="3"/>
+      <c r="BD62" s="3"/>
+      <c r="BE62" s="3"/>
+      <c r="BF62" s="3"/>
+      <c r="BG62" s="3"/>
+      <c r="BH62" s="3"/>
+      <c r="BI62" s="3"/>
+      <c r="BJ62" s="3"/>
+      <c r="BK62" s="3"/>
+      <c r="BL62" s="3"/>
+      <c r="BM62" s="3"/>
+      <c r="BN62" s="3"/>
+      <c r="BO62" s="3"/>
+      <c r="BP62" s="3"/>
+      <c r="BQ62" s="3"/>
+      <c r="BR62" s="9">
+        <v>1</v>
+      </c>
+      <c r="BS62" s="9">
+        <v>1</v>
+      </c>
+      <c r="BT62" s="9">
+        <v>1</v>
+      </c>
+      <c r="BU62" s="3"/>
+      <c r="BV62" s="3"/>
+      <c r="BW62" s="3"/>
+      <c r="BX62" s="3"/>
+      <c r="BY62" s="3"/>
+      <c r="BZ62" s="3"/>
+      <c r="CA62" s="3"/>
+      <c r="CB62" s="3"/>
+      <c r="CC62" s="3"/>
+      <c r="CD62" s="3"/>
+      <c r="CE62" s="3"/>
+      <c r="CF62" s="3"/>
+      <c r="CG62" s="3"/>
+      <c r="CH62" s="3"/>
+      <c r="CI62" s="3"/>
+      <c r="CJ62" s="3"/>
+      <c r="CK62" s="3"/>
+      <c r="CL62" s="3"/>
+      <c r="CM62" s="3"/>
+      <c r="CN62" s="3"/>
+      <c r="CO62" s="3"/>
+      <c r="CP62" s="3"/>
+      <c r="CQ62" s="3"/>
+      <c r="CR62" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="CS62" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT62" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU62" s="3"/>
+      <c r="CV62" s="3"/>
+      <c r="CW62" s="3"/>
+      <c r="CX62" s="3"/>
+      <c r="CY62" s="3"/>
+      <c r="CZ62" s="3"/>
+      <c r="DA62" s="3"/>
+      <c r="DB62" s="3"/>
+      <c r="DC62" s="3"/>
+      <c r="DD62" s="3"/>
+      <c r="DE62" s="3"/>
+      <c r="DF62" s="3"/>
+      <c r="DG62" s="3"/>
+      <c r="DH62" s="3"/>
+      <c r="DI62" s="3"/>
+      <c r="DJ62" s="3"/>
+      <c r="DK62" s="3"/>
+      <c r="DL62">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:116" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+      <c r="AA63" s="3"/>
+      <c r="AB63" s="3"/>
+      <c r="AC63" s="3"/>
+      <c r="AD63" s="3"/>
+      <c r="AE63" s="3"/>
+      <c r="AF63" s="3"/>
+      <c r="AG63" s="3"/>
+      <c r="AH63" s="3"/>
+      <c r="AI63" s="3"/>
+      <c r="AJ63" s="3"/>
+      <c r="AK63" s="3"/>
+      <c r="AL63" s="3"/>
+      <c r="AM63" s="3"/>
+      <c r="AN63" s="3"/>
+      <c r="AO63" s="3"/>
+      <c r="AP63" s="3"/>
+      <c r="AQ63" s="3"/>
+      <c r="AR63" s="3"/>
+      <c r="AS63" s="3"/>
+      <c r="AT63" s="3"/>
+      <c r="AU63" s="3"/>
+      <c r="AV63" s="3"/>
+      <c r="AW63" s="3"/>
+      <c r="AX63" s="3"/>
+      <c r="AY63" s="3"/>
+      <c r="AZ63" s="3"/>
+      <c r="BA63" s="3"/>
+      <c r="BB63" s="3"/>
+      <c r="BC63" s="3"/>
+      <c r="BD63" s="3"/>
+      <c r="BE63" s="3"/>
+      <c r="BF63" s="3"/>
+      <c r="BG63" s="3"/>
+      <c r="BH63" s="3"/>
+      <c r="BI63" s="3"/>
+      <c r="BJ63" s="3"/>
+      <c r="BK63" s="3"/>
+      <c r="BL63" s="3"/>
+      <c r="BM63" s="3"/>
+      <c r="BN63" s="3"/>
+      <c r="BO63" s="3"/>
+      <c r="BP63" s="3"/>
+      <c r="BQ63" s="3"/>
+      <c r="BR63" s="8"/>
+      <c r="BS63" s="8"/>
+      <c r="BT63" s="8"/>
+      <c r="BU63" s="3"/>
+      <c r="BV63" s="3"/>
+      <c r="BW63" s="3"/>
+      <c r="BX63" s="3"/>
+      <c r="BY63" s="3"/>
+      <c r="BZ63" s="4">
+        <v>1</v>
+      </c>
+      <c r="CA63" s="3"/>
+      <c r="CB63" s="3"/>
+      <c r="CC63" s="3"/>
+      <c r="CD63" s="3"/>
+      <c r="CE63" s="3"/>
+      <c r="CF63" s="3"/>
+      <c r="CG63" s="3"/>
+      <c r="CH63" s="3"/>
+      <c r="CI63" s="3"/>
+      <c r="CJ63" s="3"/>
+      <c r="CK63" s="3"/>
+      <c r="CL63" s="3"/>
+      <c r="CM63" s="3"/>
+      <c r="CN63" s="3"/>
+      <c r="CO63" s="3"/>
+      <c r="CP63" s="3"/>
+      <c r="CQ63" s="3"/>
+      <c r="CR63" s="3"/>
+      <c r="CS63" s="3"/>
+      <c r="CT63" s="3"/>
+      <c r="CU63" s="3"/>
+      <c r="CV63" s="3"/>
+      <c r="CW63" s="3"/>
+      <c r="CX63" s="3"/>
+      <c r="CY63" s="3"/>
+      <c r="CZ63" s="3"/>
+      <c r="DA63" s="3"/>
+      <c r="DB63" s="3"/>
+      <c r="DC63" s="3"/>
+      <c r="DD63" s="3"/>
+      <c r="DE63" s="3"/>
+      <c r="DF63" s="3"/>
+      <c r="DG63" s="3"/>
+      <c r="DH63" s="3"/>
+      <c r="DI63" s="3"/>
+      <c r="DJ63" s="3"/>
+      <c r="DK63" s="3"/>
+      <c r="DL63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="89:89" x14ac:dyDescent="0.3">
       <c r="CK65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -8449,6 +9259,11 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B3:DK63">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>